<commit_message>
Add Bento MenopauseStatus, PRStatus, Program suites
</commit_message>
<xml_diff>
--- a/InputFiles/Bento/TC01_Bento_Filter_MenoStatus-Post.xlsx
+++ b/InputFiles/Bento/TC01_Bento_Filter_MenoStatus-Post.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sohilz2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leungvw/git/Commons_Automation/InputFiles/Bento/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749D0B4C-8A7D-46FA-8798-8C064F17C7DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22EEEEBA-7D8F-2844-9FA9-033E7E54A44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16354" yWindow="-4860" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
+    <workbookView xWindow="2900" yWindow="-25540" windowWidth="33120" windowHeight="18120" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
   <sheets>
     <sheet name="startup" sheetId="1" r:id="rId1"/>
@@ -31,17 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>WebExcel</t>
   </si>
   <si>
-    <t>query</t>
-  </si>
-  <si>
-    <t>dbExcel</t>
-  </si>
-  <si>
     <t>StatQuery</t>
   </si>
   <si>
@@ -51,28 +45,6 @@
     <t>CasesTab</t>
   </si>
   <si>
-    <t>MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
-   WHERE    demo.menopause_status IN ["Postmenopausal"] 
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(samp)
-MATCH (samp)&lt;-[:file_of_sample]-(f)
-MATCH (lp)&lt;-[:file_of_laboratory_procedure]-(f)
-RETURN COUNT(DISTINCT p) AS Programs,
-COUNT(DISTINCT s) AS Arms,
-COUNT(DISTINCT ss) AS Cases,
-COUNT(DISTINCT samp) AS Samples,
-COUNT(DISTINCT lp) AS Assays,
-COUNT(DISTINCT f) AS Files</t>
-  </si>
-  <si>
-    <t>TC01_Bento_Filter_MenoStatus-Post_Neo4jData.xlsx</t>
-  </si>
-  <si>
     <t>TC01_Bento_Filter_MenoStatus-Post_WebData.xlsx</t>
   </si>
   <si>
@@ -82,99 +54,236 @@
     <t>FilesTab</t>
   </si>
   <si>
-    <t xml:space="preserve">MATCH (ss:study_subject)
-MATCH (ss)&lt;-[:sample_of_study_subject]-(sp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-WITH ss, collect(DISTINCT sp.sample_id) AS samples, collect(DISTINCT lp.laboratory_procedure_id) AS lab_procedures, collect(DISTINCT f) AS files
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
-MATCH (ss)&lt;-[:sf_of_study_subject]-(sf)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
-   WHERE    demo.menopause_status IN ["Postmenopausal"] 
-return ss.study_subject_id as `Case ID`,
-       p.program_acronym as `Program Code`,
-        p.program_id as Program_ID,
-       s.study_acronym as `Arm`,
-       ss.disease_subtype as `Diagnosis`,
-       sf.grouped_recurrence_score AS `Recurrence Score`,
-       d.tumor_size_group AS `tumor_size`,
-       d.er_status AS `ER Status`,
-       d.pr_status AS `PR Status`,
-       coalesce(CASE demo.age_at_index % 1 WHEN 0 THEN apoc.convert.toInteger(demo.age_at_index) ELSE demo.age_at_index END, '') AS `Age (years)`,
-       demo.survival_time AS `Survival (days)`
-   order By ss.study_subject_id ASC LIMIT 100 </t>
-  </si>
-  <si>
-    <t>MATCH (ss:study_subject)
-WITH COLLECT(ss.study_subject_id) AS all_subjects
-MATCH (samp:sample)
-MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)-[:study_of_program]-&gt;(p)
-MATCH (samp)&lt;-[:file_of_sample]-(f)-[:file_of_laboratory_procedure]-&gt;(lp)
-MATCH (ss)&lt;-[:diagnosis_of_study_subject]-(d)
-MATCH (d)&lt;-[:tp_of_diagnosis]-(tp)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
-WHERE    demo.menopause_status IN ["Postmenopausal"] 
-WITH
-    distinct lp,
-    toInteger(split(ss.study_subject_id,'-')[2]) AS subject_id_num,
-    collect(distinct f.file_id) AS files,
-    samp, ss, s, p, all_subjects
-RETURN
- samp.sample_id AS `Sample ID`,
-            ss.study_subject_id AS `Case ID`,
-            p.program_acronym AS `Program Code`,
-            s.study_acronym AS `Arm`,
-            ss.disease_subtype AS `Diagnosis`,
-            samp.tissue_type AS `Tissue Type`,
-            samp.composition AS `Tissue Composition`,
-            samp.sample_anatomic_site AS `Sample Anatomic Site`,
-            samp.method_of_sample_procurement AS `Sample Procurement Method`
- order By samp.sample_id ASC LIMIT 100</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)--&gt;(parent)
-MATCH (f)-[:file_of_sample]-&gt;(samp)
-MATCH (samp)-[:sample_of_study_subject]-&gt;(ss)
-MATCH (ss)-[:study_subject_of_study]-&gt;(s)
-MATCH (s)-[:study_of_program]-&gt;(p)
-MATCH (d)-[:diagnosis_of_study_subject]-&gt;(ss)
-MATCH (tp)-[:tp_of_diagnosis]-&gt;(d)
-MATCH (ss)&lt;-[:demographic_of_study_subject]-(demo)
-WHERE demo.menopause_status IN ["Postmenopausal"] 
-WITH
-        f, demo,parent,p, ss, d,tp, s, samp,
-        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
-        toInteger(floor(log(f.file_size)/log(1024))) as i,
-        2 as precision
-WITH
-        f, parent,p, ss, d,tp, s, samp,
-        f.file_size /(1024^i) AS value,
-        10^precision AS factor,
-        units[i] as unit
-WITH
-        f, parent,p, ss, d,tp, s, samp, unit,
-        round(factor * value)/factor AS size
-RETURN Distinct
-    f.file_name AS `File Name`,
-    head(labels(samp)) AS `Association`,
-    f.file_description AS `Description`,
-    f.file_format AS `File Format`,
-    CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
-    p.program_acronym AS `Program Code`,
-    s.study_acronym AS `Arm`,
-    ss.study_subject_id AS `Case ID`,
-    samp.sample_id AS `Sample ID`
- order By f.file_name ASC LIMIT 100</t>
+    <t>TabQuery</t>
+  </si>
+  <si>
+    <t>TsvExcel</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    sts.study_subject_id AS "Case ID",
+    prg.program_acronym AS "Program Code",
+    prg.program_id AS "Program ID",
+    std.study_acronym AS "ARM",
+    sts.disease_subtype AS "Diagnosis",
+    stf.grouped_recurrence_score AS "Recurrence Score",
+    dgn.tumor_size_group AS "Tumor Size (cm)",
+    dgn.er_status AS "ER Status",
+    dgn.pr_status AS "PR Status",
+    dem.age_at_index AS "Age (years)",
+    CASE 
+        WHEN dem.survival_time = 0 THEN ''
+        ELSE dem.survival_time
+    END AS "Survival (days)"
+FROM 
+    df_program prg
+LEFT JOIN 
+    df_study std ON prg.program_id = std."program.program_id"
+LEFT JOIN 
+    df_study_subject sts ON std.study_id = sts."study.study_id"
+LEFT JOIN
+    df_diagnosis dgn ON sts.study_subject_id = dgn."study_subject.study_subject_id"
+LEFT JOIN
+    df_stratification_factor stf ON sts.study_subject_id = stf."study_subject.study_subject_id"
+LEFT JOIN
+    df_demographic_data dem ON sts.study_subject_id = dem."study_subject.study_subject_id"
+LEFT JOIN
+    df_therapeutic_procedure tpp ON dgn.diagnosis_id = tpp."diagnosis.diagnosis_id"
+LEFT JOIN
+    df_sample smp ON sts.study_subject_id = smp."study_subject.study_subject_id"
+WHERE 
+    dem.menopause_status = 'Postmenopausal'
+ORDER BY 
+    sts.study_subject_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    smp.sample_id AS "Sample ID",
+    sts.study_subject_id AS "Case ID",
+    prg.program_acronym AS "Program Code",
+    std.study_acronym AS "ARM",
+    sts.disease_subtype AS "Diagnosis",
+    smp.tissue_type AS "Tissue Type",
+    smp.composition AS "Tissue Composition",
+    smp.sample_anatomic_site AS "Sample Anatomic Site",
+    smp.method_of_sample_procurement AS "Sample Procurement Method",
+    lab.test_name AS "platform"
+FROM 
+    df_program prg
+LEFT JOIN 
+    df_study std ON prg.program_id = std."program.program_id"
+LEFT JOIN 
+    df_study_subject sts ON std.study_id = sts."study.study_id"
+LEFT JOIN
+    df_diagnosis dgn ON sts.study_subject_id = dgn."study_subject.study_subject_id"
+LEFT JOIN
+    df_stratification_factor stf ON sts.study_subject_id = stf."study_subject.study_subject_id"
+LEFT JOIN
+    df_demographic_data dem ON sts.study_subject_id = dem."study_subject.study_subject_id"
+LEFT JOIN
+    df_sample smp ON sts.study_subject_id = smp."study_subject.study_subject_id"
+LEFT JOIN
+    df_laboratory_procedure lab ON prg.program_id = lab."program.program_id"
+LEFT JOIN
+    df_file fil ON smp.sample_id = fil."sample.sample_id"
+LEFT JOIN
+    df_therapeutic_procedure tpp ON dgn.diagnosis_id = tpp."diagnosis.diagnosis_id"
+WHERE 
+    dem.menopause_status = 'Postmenopausal'
+ORDER BY 
+    smp.sample_id ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT DISTINCT
+    file_name AS "File Name",
+    sample_type AS "Association",
+    file_description AS "Description",
+    file_format AS "File Format",
+    CASE 
+        WHEN file_size &gt;= 1073741824  
+            THEN ROUND(file_size / 1073741824.0, 2) || ' GB'
+        WHEN file_size &gt;= 1048576  
+            THEN ROUND(file_size / 1048576.0, 2) || ' MB'
+        WHEN file_size &gt;= 1024  
+            THEN ROUND(file_size / 1024.0, 2) || ' KB'
+        ELSE file_size || ' Bytes'
+    END AS "Size",
+    program_acronym AS "Program Code",
+    study_acronym AS "ARM",
+    study_subject_id AS "Case ID",
+    sample_id AS "Sample ID"
+FROM (
+    SELECT fil.file_name, smp.type AS sample_type, fil.file_description, fil.file_format, 
+           fil.file_size, prg.program_acronym, std.study_acronym, sts.study_subject_id, smp.sample_id
+    FROM df_file fil
+    JOIN df_sample smp ON fil."sample.sample_id" = smp.sample_id
+    JOIN df_study_subject sts ON smp."study_subject.study_subject_id" = sts.study_subject_id
+    JOIN df_study std ON sts."study.study_id" = std.study_id
+    JOIN df_program prg ON std."program.program_id" = prg.program_id
+    JOIN df_diagnosis dgn ON sts.study_subject_id = dgn."study_subject.study_subject_id"
+    JOIN df_therapeutic_procedure tpp ON dgn.diagnosis_id = tpp."diagnosis.diagnosis_id"
+    JOIN df_demographic_data dem ON sts.study_subject_id = dem."study_subject.study_subject_id"
+    WHERE dem.menopause_status = 'Postmenopausal'
+    UNION  
+    SELECT vcf.file_name, smp.type, vcf.file_description, vcf.file_format, 
+           vcf.file_size, prg.program_acronym, std.study_acronym, sts.study_subject_id, smp.sample_id
+    FROM df_file_vcf vcf
+    JOIN df_sample smp ON vcf."sample.sample_id" = smp.sample_id
+    JOIN df_study_subject sts ON smp."study_subject.study_subject_id" = sts.study_subject_id
+    JOIN df_study std ON sts."study.study_id" = std.study_id
+    JOIN df_program prg ON std."program.program_id" = prg.program_id
+    JOIN df_diagnosis dgn ON sts.study_subject_id = dgn."study_subject.study_subject_id"
+    JOIN df_therapeutic_procedure tpp ON dgn.diagnosis_id = tpp."diagnosis.diagnosis_id"
+    JOIN df_demographic_data dem ON sts.study_subject_id = dem."study_subject.study_subject_id"
+    WHERE dem.menopause_status = 'Postmenopausal'
+    UNION  
+    SELECT bam.file_name, smp.type, bam.file_description, bam.file_format, 
+           bam.file_size, prg.program_acronym, std.study_acronym, sts.study_subject_id, smp.sample_id
+    FROM df_file_bam bam
+    JOIN df_sample smp ON bam."sample.sample_id" = smp.sample_id
+    JOIN df_study_subject sts ON smp."study_subject.study_subject_id" = sts.study_subject_id
+    JOIN df_study std ON sts."study.study_id" = std.study_id
+    JOIN df_program prg ON std."program.program_id" = prg.program_id
+    JOIN df_diagnosis dgn ON sts.study_subject_id = dgn."study_subject.study_subject_id"
+    JOIN df_therapeutic_procedure tpp ON dgn.diagnosis_id = tpp."diagnosis.diagnosis_id"
+    JOIN df_demographic_data dem ON sts.study_subject_id = dem."study_subject.study_subject_id"
+    WHERE dem.menopause_status = 'Postmenopausal'
+) AS combined_files
+ORDER BY "File Name" ASC
+LIMIT 100;</t>
+  </si>
+  <si>
+    <t>SELECT 
+    COUNT(DISTINCT prg.program_id) AS Programs,
+    COUNT(DISTINCT std.study_acronym) AS Arms,
+    COUNT(DISTINCT sts.study_subject_id) AS Cases,
+    COUNT(DISTINCT smp.sample_id) AS Samples,
+    COUNT(DISTINCT lab.laboratory_procedure_id) AS Assays,
+  (SELECT COUNT(DISTINCT file_id) FROM (
+    SELECT fil.file_id 
+    FROM df_file fil
+    JOIN df_sample smp ON fil."sample.sample_id" = smp.sample_id
+    JOIN df_study_subject sts ON smp."study_subject.study_subject_id" = sts.study_subject_id
+    JOIN df_study std ON sts."study.study_id" = std.study_id
+    JOIN df_diagnosis dgn ON sts.study_subject_id = dgn."study_subject.study_subject_id"
+    JOIN df_therapeutic_procedure tpp ON dgn.diagnosis_id = tpp."diagnosis.diagnosis_id"
+    JOIN df_demographic_data dem ON sts.study_subject_id = dem."study_subject.study_subject_id"
+    WHERE dem.menopause_status = 'Postmenopausal'
+    UNION  
+    SELECT vcf.file_id 
+    FROM df_file_vcf vcf
+    JOIN df_sample smp ON vcf."sample.sample_id" = smp.sample_id
+    JOIN df_study_subject sts ON smp."study_subject.study_subject_id" = sts.study_subject_id
+    JOIN df_study std ON sts."study.study_id" = std.study_id
+    JOIN df_diagnosis dgn ON sts.study_subject_id = dgn."study_subject.study_subject_id"
+    JOIN df_therapeutic_procedure tpp ON dgn.diagnosis_id = tpp."diagnosis.diagnosis_id"
+    JOIN df_demographic_data dem ON sts.study_subject_id = dem."study_subject.study_subject_id"
+    WHERE dem.menopause_status = 'Postmenopausal'
+    UNION  
+    SELECT bam.file_id 
+    FROM df_file_bam bam
+    JOIN df_sample smp ON bam."sample.sample_id" = smp.sample_id
+    JOIN df_study_subject sts ON smp."study_subject.study_subject_id" = sts.study_subject_id
+    JOIN df_study std ON sts."study.study_id" = std.study_id
+    JOIN df_diagnosis dgn ON sts.study_subject_id = dgn."study_subject.study_subject_id"
+    JOIN df_therapeutic_procedure tpp ON dgn.diagnosis_id = tpp."diagnosis.diagnosis_id"
+    JOIN df_demographic_data dem ON sts.study_subject_id = dem."study_subject.study_subject_id"
+    WHERE dem.menopause_status = 'Postmenopausal'
+ ) AS filtered_files) AS Files
+FROM 
+    df_program prg
+LEFT JOIN 
+    df_study std ON prg.program_id = std."program.program_id"
+LEFT JOIN 
+    df_study_subject sts ON std.study_id = sts."study.study_id"
+LEFT JOIN
+    df_diagnosis dgn ON sts.study_subject_id = dgn."study_subject.study_subject_id"
+LEFT JOIN
+    df_stratification_factor stf ON sts.study_subject_id = stf."study_subject.study_subject_id"
+LEFT JOIN
+    df_demographic_data dem ON sts.study_subject_id = dem."study_subject.study_subject_id"
+LEFT JOIN
+    df_sample smp ON sts.study_subject_id = smp."study_subject.study_subject_id"
+LEFT JOIN
+    df_laboratory_procedure lab ON prg.program_id = lab."program.program_id"
+LEFT JOIN
+    df_file fil ON smp.sample_id = fil."sample.sample_id"
+LEFT JOIN
+    df_file_vcf vcf ON smp.sample_id = vcf."sample.sample_id"
+LEFT JOIN
+    df_file_bam bam ON smp.sample_id = bam."sample.sample_id"
+LEFT JOIN
+    df_therapeutic_procedure tpp ON dgn.diagnosis_id = tpp."diagnosis.diagnosis_id"
+WHERE 
+    dem.menopause_status = 'Postmenopausal'</t>
+  </si>
+  <si>
+    <t>TC01_Bento_Filter_MenoStatus-Post_TsvData.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -213,11 +322,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -239,9 +351,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -279,7 +391,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -385,7 +497,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -527,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -537,89 +649,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.77734375" customWidth="1"/>
-    <col min="3" max="3" width="60.44140625" customWidth="1"/>
-    <col min="4" max="4" width="70.21875" customWidth="1"/>
-    <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86.83203125" customWidth="1"/>
+    <col min="3" max="3" width="83.33203125" customWidth="1"/>
+    <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="360" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="374.4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
+      <c r="C4" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>